<commit_message>
adding recursive standards and subject numbers
</commit_message>
<xml_diff>
--- a/data/subjects/all_subjects.xlsx
+++ b/data/subjects/all_subjects.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="4720" windowWidth="28800" windowHeight="16700" tabRatio="789" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="1320" yWindow="80" windowWidth="25600" windowHeight="16060" tabRatio="789" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ELA" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="518">
   <si>
     <t>English Language Arts</t>
   </si>
@@ -129,27 +129,6 @@
   </si>
   <si>
     <t>Modern World</t>
-  </si>
-  <si>
-    <t>sources</t>
-  </si>
-  <si>
-    <t>http://www.nchs.ucla.edu/Standards/Standards</t>
-  </si>
-  <si>
-    <t>http://www.socialstudies.org/c3</t>
-  </si>
-  <si>
-    <t>http://www.cde.ca.gov/be/st/ss/documents/histsocscistnd.pdf</t>
-  </si>
-  <si>
-    <t>might further use…</t>
-  </si>
-  <si>
-    <t>nation</t>
-  </si>
-  <si>
-    <t>http://education.nationalgeographic.com/education/national-geography-standards/?ar_a=1</t>
   </si>
   <si>
     <t>Maps and Geographic Representations</t>
@@ -2492,372 +2471,372 @@
     </row>
     <row r="2" spans="1:5">
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="C3" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="D4" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="D5" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="D6" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="D7" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="C8" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="E9" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="E10" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="E11" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="E12" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="E13" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="E14" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="E15" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="E16" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="E17" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="E18" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:5">
       <c r="E19" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="E20" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="C21" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="E22" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="2:5">
       <c r="E23" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="2:5">
       <c r="E24" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="2:5">
       <c r="E25" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="2:5">
       <c r="C27" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="2:5">
       <c r="D28" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="2:5">
       <c r="D29" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="2:5">
       <c r="D30" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="2:5">
       <c r="D31" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="2:5">
       <c r="D32" s="2" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
     </row>
     <row r="33" spans="3:5">
       <c r="D33" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="3:5">
       <c r="D34" s="2" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
     </row>
     <row r="35" spans="3:5">
       <c r="D35" s="2" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
     </row>
     <row r="36" spans="3:5">
       <c r="C36" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="3:5">
       <c r="D37" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="3:5">
       <c r="E38" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="3:5">
       <c r="E39" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="3:5">
       <c r="E40" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="3:5">
       <c r="E41" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="3:5">
       <c r="D42" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="3:5">
       <c r="E43" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="3:5">
       <c r="E44" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="3:5">
       <c r="E45" s="2" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
     </row>
     <row r="46" spans="3:5">
       <c r="C46" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="3:5">
       <c r="D47" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="3:5">
       <c r="D48" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="2:4">
       <c r="D49" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="2:4">
       <c r="D50" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="2:4">
       <c r="D51" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="D52" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="2:4">
       <c r="D53" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="2:4">
       <c r="D54" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="2:4">
       <c r="C55" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="2:4">
       <c r="D56" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="2:4">
       <c r="D57" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="2:4">
       <c r="D58" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="B59" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="2:4">
       <c r="C60" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="2:4">
       <c r="D61" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="2:4">
       <c r="D62" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="2:4">
       <c r="D63" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="C64" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="D65" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="D66" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="D67" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="D69" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="D70" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="D72" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="D73" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="D74" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="D75" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2875,7 +2854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -2883,32 +2862,32 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="B2" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2933,152 +2912,152 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="B2" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="C3" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="C4" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="C5" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="C6" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="C7" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="C8" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="C9" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="C10" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="C11" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="C12" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="C13" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="C14" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="C15" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="B16" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="B19" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="B20" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="C23" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="C24" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="C25" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
     </row>
     <row r="26" spans="2:3">
       <c r="B26" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
     </row>
     <row r="27" spans="2:3">
       <c r="C27" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
     </row>
     <row r="28" spans="2:3">
       <c r="C28" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
     </row>
     <row r="29" spans="2:3">
       <c r="B29" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
     </row>
     <row r="30" spans="2:3">
       <c r="B30" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -3103,257 +3082,257 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="B2" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="C3" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="C4" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="C5" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="C6" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="C7" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="B8" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="C9" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="C10" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="C11" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="C12" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="C13" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="C15" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="C16" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="C17" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="C18" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="C19" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="C20" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="C21" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="C22" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="C23" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="C24" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="C25" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="26" spans="2:3">
       <c r="B26" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="27" spans="2:3">
       <c r="C27" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="28" spans="2:3">
       <c r="C28" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="29" spans="2:3">
       <c r="C29" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
     </row>
     <row r="30" spans="2:3">
       <c r="C30" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" spans="2:3">
       <c r="C31" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
     </row>
     <row r="32" spans="2:3">
       <c r="C32" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="34" spans="2:3">
       <c r="C34" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="C35" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
     </row>
     <row r="36" spans="2:3">
       <c r="C36" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
     </row>
     <row r="37" spans="2:3">
       <c r="B37" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="38" spans="2:3">
       <c r="C38" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="39" spans="2:3">
       <c r="C39" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
     </row>
     <row r="40" spans="2:3">
       <c r="C40" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="41" spans="2:3">
       <c r="B41" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="42" spans="2:3">
       <c r="C42" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
     </row>
     <row r="43" spans="2:3">
       <c r="C43" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="44" spans="2:3">
       <c r="C44" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
     </row>
     <row r="45" spans="2:3">
       <c r="B45" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
     </row>
     <row r="46" spans="2:3">
       <c r="C46" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="47" spans="2:3">
       <c r="C47" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
     </row>
     <row r="48" spans="2:3">
       <c r="C48" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
     </row>
     <row r="49" spans="3:3">
       <c r="C49" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
     </row>
     <row r="50" spans="3:3">
       <c r="C50" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="51" spans="3:3">
       <c r="C51" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>
@@ -3384,507 +3363,507 @@
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="C3" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="C4" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="C6" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="D7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="D8" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="D9" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="D10" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="D11" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="C12" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="D13" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="E14" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="E15" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="D16" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="E17" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="E18" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
     </row>
     <row r="19" spans="2:5">
       <c r="E19" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="E20" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="C22" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="2:5">
       <c r="C23" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="2:5">
       <c r="C24" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="2:5">
       <c r="C25" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="2:5">
       <c r="C26" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="2:5">
       <c r="C27" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="2:5">
       <c r="C29" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="2:5">
       <c r="D30" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
     </row>
     <row r="31" spans="2:5">
       <c r="D31" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
     </row>
     <row r="32" spans="2:5">
       <c r="D32" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="D33" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="D34" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="C35" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="2:4">
       <c r="C36" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="C37" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="C38" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="2:4">
       <c r="C39" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="C40" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="C43" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="2:4">
       <c r="C44" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="2:4">
       <c r="C45" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="2:4">
       <c r="C46" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="C48" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="2:3">
       <c r="C49" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="2:3">
       <c r="C50" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="2:3">
       <c r="C51" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="2:3">
       <c r="C52" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="2:3">
       <c r="C53" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="2:3">
       <c r="C54" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="2:3">
       <c r="C55" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="2:3">
       <c r="B56" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="2:3">
       <c r="C57" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="2:3">
       <c r="C58" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="2:3">
       <c r="C59" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="2:3">
       <c r="C60" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="2:3">
       <c r="C61" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="2:3">
       <c r="C62" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="2:3">
       <c r="B63" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="2:3">
       <c r="C64" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" spans="2:3">
       <c r="C65" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="66" spans="2:3">
       <c r="C66" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="2:3">
       <c r="C67" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="68" spans="2:3">
       <c r="C68" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="69" spans="2:3">
       <c r="B69" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="2:3">
       <c r="C70" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" spans="2:3">
       <c r="C71" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="72" spans="2:3">
       <c r="C72" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="73" spans="2:3">
       <c r="C73" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="2:3">
       <c r="C74" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="75" spans="2:3">
       <c r="C75" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" spans="2:3">
       <c r="C76" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="77" spans="2:3">
       <c r="C77" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="78" spans="2:3">
       <c r="B78" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" spans="2:3">
       <c r="C79" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="80" spans="2:3">
       <c r="C80" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="81" spans="2:4">
       <c r="C81" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="82" spans="2:4">
       <c r="C82" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="83" spans="2:4">
       <c r="C83" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="84" spans="2:4">
       <c r="C84" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="85" spans="2:4">
       <c r="D85" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="86" spans="2:4">
       <c r="D86" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="87" spans="2:4">
       <c r="D87" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="88" spans="2:4">
       <c r="D88" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
     </row>
     <row r="89" spans="2:4">
       <c r="C89" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
     </row>
     <row r="90" spans="2:4">
       <c r="C90" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="91" spans="2:4">
       <c r="B91" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="92" spans="2:4">
       <c r="C92" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="93" spans="2:4">
       <c r="C93" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
     </row>
     <row r="94" spans="2:4">
       <c r="C94" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="95" spans="2:4">
       <c r="C95" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="96" spans="2:4">
       <c r="C96" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="97" spans="2:3">
       <c r="B97" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="98" spans="2:3">
       <c r="C98" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="99" spans="2:3">
       <c r="C99" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
     </row>
     <row r="100" spans="2:3">
       <c r="C100" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="101" spans="2:3">
       <c r="C101" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="102" spans="2:3">
       <c r="C102" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="103" spans="2:3">
       <c r="C103" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -3910,472 +3889,472 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="C3" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="D4" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="D5" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="D6" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="D7" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="D8" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="D9" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="D10" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="C12" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="D13" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="D14" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="D15" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="D16" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="3:4">
       <c r="D17" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="3:4">
       <c r="D18" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="3:4">
       <c r="D19" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="3:4">
       <c r="C20" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="3:4">
       <c r="D21" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="3:4">
       <c r="D22" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="3:4">
       <c r="D23" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="3:4">
       <c r="D24" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="3:4">
       <c r="D25" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="3:4">
       <c r="D26" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="3:4">
       <c r="D27" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="3:4">
       <c r="D28" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" spans="3:4">
       <c r="D29" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="3:4">
       <c r="D30" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="3:4">
       <c r="D31" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="3:4">
       <c r="C32" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="4:6">
       <c r="D33" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="4:6">
       <c r="E34" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="4:6">
       <c r="E35" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="4:6">
       <c r="E36" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="4:6">
       <c r="E37" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="4:6">
       <c r="E38" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="4:6">
       <c r="E39" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="4:6">
       <c r="E40" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41" spans="4:6">
       <c r="D41" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="4:6">
       <c r="E43" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="4:6">
       <c r="E44" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="4:6">
       <c r="F45" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="4:6">
       <c r="F46" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="4:6">
       <c r="D47" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="4:6">
       <c r="E48" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="49" spans="2:4">
       <c r="D49" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="50" spans="2:4">
       <c r="D50" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="51" spans="2:4">
       <c r="D51" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="D52" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="54" spans="2:4">
       <c r="C54" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="2:4">
       <c r="D55" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" spans="2:4">
       <c r="D56" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="57" spans="2:4">
       <c r="D57" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="2:4">
       <c r="D58" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="C59" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="60" spans="2:4">
       <c r="D60" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61" spans="2:4">
       <c r="D61" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="2:4">
       <c r="D62" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="63" spans="2:4">
       <c r="D63" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="D64" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="65" spans="2:4">
       <c r="D65" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="66" spans="2:4">
       <c r="C66" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="67" spans="2:4">
       <c r="D67" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="68" spans="2:4">
       <c r="D68" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="69" spans="2:4">
       <c r="D69" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="70" spans="2:4">
       <c r="D70" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="71" spans="2:4">
       <c r="D71" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="72" spans="2:4">
       <c r="D72" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="73" spans="2:4">
       <c r="D73" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="74" spans="2:4">
       <c r="C74" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="75" spans="2:4">
       <c r="D75" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="76" spans="2:4">
       <c r="C76" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="77" spans="2:4">
       <c r="C77" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
     <row r="78" spans="2:4">
       <c r="B78" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="79" spans="2:4">
       <c r="C79" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="80" spans="2:4">
       <c r="D80" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="81" spans="2:5">
       <c r="D81" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="82" spans="2:5">
       <c r="D82" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="83" spans="2:5">
       <c r="D83" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="84" spans="2:5">
       <c r="D84" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="85" spans="2:5">
       <c r="E85" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="86" spans="2:5">
       <c r="E86" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="87" spans="2:5">
       <c r="C87" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="88" spans="2:5">
       <c r="D88" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="89" spans="2:5">
       <c r="D89" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="90" spans="2:5">
       <c r="D90" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="91" spans="2:5">
       <c r="D91" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="93" spans="2:5">
       <c r="B93" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="94" spans="2:5">
       <c r="C94" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="95" spans="2:5">
       <c r="C95" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="96" spans="2:5">
       <c r="C96" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -4391,17 +4370,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4456,17 +4435,17 @@
     </row>
     <row r="13" spans="1:4">
       <c r="C13" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="D14" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="D15" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4476,17 +4455,17 @@
     </row>
     <row r="17" spans="3:5">
       <c r="E17" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="3:5">
       <c r="E18" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="3:5">
       <c r="E19" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="3:5">
@@ -4496,32 +4475,32 @@
     </row>
     <row r="21" spans="3:5">
       <c r="D21" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="3:5">
       <c r="D22" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="3:5">
       <c r="D23" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="3:5">
       <c r="D24" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="3:5">
       <c r="D25" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="3:5">
       <c r="D26" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="3:5">
@@ -4531,17 +4510,17 @@
     </row>
     <row r="30" spans="3:5">
       <c r="D30" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="3:5">
       <c r="D31" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="3:5">
       <c r="D32" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="2:5">
@@ -4551,17 +4530,17 @@
     </row>
     <row r="35" spans="2:5">
       <c r="D35" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="E36" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="E37" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="2:5">
@@ -4571,7 +4550,7 @@
     </row>
     <row r="39" spans="2:5">
       <c r="E39" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="2:5">
@@ -4619,70 +4598,39 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="3:12">
+    <row r="49" spans="3:4">
       <c r="D49" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="3:12">
+    <row r="50" spans="3:4">
       <c r="D50" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="3:12">
+    <row r="52" spans="3:4">
       <c r="C52" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="3:12">
+    <row r="53" spans="3:4">
       <c r="D53" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="3:12">
+    <row r="54" spans="3:4">
       <c r="D54" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="3:12">
+    <row r="55" spans="3:4">
       <c r="D55" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="3:12">
+    <row r="56" spans="3:4">
       <c r="D56" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="57" spans="3:12">
-      <c r="H57" t="s">
-        <v>33</v>
-      </c>
-      <c r="J57" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="58" spans="3:12">
-      <c r="H58" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="59" spans="3:12">
-      <c r="H59" t="s">
-        <v>34</v>
-      </c>
-      <c r="L59" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="60" spans="3:12">
-      <c r="H60" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="61" spans="3:12">
-      <c r="H61" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -4707,127 +4655,127 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="B2" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="B7" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="B11" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="B12" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="B15" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="B16" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -4844,7 +4792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
@@ -4852,192 +4800,192 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="B2" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="C3" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="C4" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="C5" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="C6" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="C7" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="B8" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="C9" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="C10" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="C11" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="C12" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="C13" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="C15" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="C16" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="C17" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="D18" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="D19" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="D20" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="D21" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="C22" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="C23" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="C24" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="C25" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="C26" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="C28" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="C29" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="C30" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="C31" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="C32" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="33" spans="3:3">
       <c r="C33" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
     </row>
     <row r="34" spans="3:3">
       <c r="C34" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
     <row r="35" spans="3:3">
       <c r="C35" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
     </row>
     <row r="36" spans="3:3">
       <c r="C36" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
     </row>
     <row r="37" spans="3:3">
       <c r="C37" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
     </row>
     <row r="38" spans="3:3">
       <c r="C38" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -5063,132 +5011,132 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="B2" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="C3" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="C4" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="C5" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="C6" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="C7" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="C8" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="C9" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="C10" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="C11" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="C12" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="C13" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="C14" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="C15" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="C16" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="C17" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="C18" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="B19" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="B20" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="C23" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="C24" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="B25" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
     </row>
     <row r="26" spans="2:3">
       <c r="B26" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
     </row>
   </sheetData>
@@ -5214,92 +5162,92 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="B2" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="C3" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="C4" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="B6" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="C7" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="C8" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="B10" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="C11" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="C12" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="C15" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="C16" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -5325,57 +5273,57 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="B2" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="B7" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="B11" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>